<commit_message>
Fixed bugs in expanded outlier_stats (outlier_all_stats); still needs more testing
</commit_message>
<xml_diff>
--- a/tables/outlier_all_stats_test.xlsx
+++ b/tables/outlier_all_stats_test.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="31">
   <si>
     <t>REGNO_SHORT</t>
   </si>
@@ -102,6 +102,21 @@
   </si>
   <si>
     <t>N</t>
+  </si>
+  <si>
+    <t>SITE_TYPE</t>
+  </si>
+  <si>
+    <t>AI_RATE_TYPE</t>
+  </si>
+  <si>
+    <t>ALL</t>
+  </si>
+  <si>
+    <t>NORMAL</t>
+  </si>
+  <si>
+    <t>OTHER</t>
   </si>
 </sst>
 </file>
@@ -125,7 +140,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -133,13 +148,47 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -420,11 +469,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O15"/>
+  <dimension ref="A1:AC15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="C39" sqref="C39"/>
+      <selection pane="bottomLeft" activeCell="Z6" sqref="Z6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -433,14 +482,19 @@
     <col min="2" max="2" width="4.140625" customWidth="1"/>
     <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="4.7109375" customWidth="1"/>
-    <col min="5" max="5" width="7.7109375" customWidth="1"/>
-    <col min="6" max="6" width="11.7109375" customWidth="1"/>
-    <col min="7" max="11" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="14" width="12.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="19.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="3.5703125" customWidth="1"/>
+    <col min="6" max="6" width="5.85546875" customWidth="1"/>
+    <col min="7" max="7" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.7109375" style="1" customWidth="1"/>
+    <col min="9" max="13" width="10.85546875" style="1" customWidth="1"/>
+    <col min="14" max="14" width="12.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="10.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="14.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="27" max="28" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -451,43 +505,73 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="Q1" s="2" t="s">
         <v>14</v>
       </c>
+      <c r="R1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -498,43 +582,93 @@
         <v>17</v>
       </c>
       <c r="D2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E2" t="s">
         <v>16</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>2171</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="G2" s="1">
-        <v>-1.1205216008225001</v>
-      </c>
-      <c r="H2" s="1">
-        <v>-0.40283692808249999</v>
+      <c r="H2" s="1" t="s">
+        <v>29</v>
       </c>
       <c r="I2" s="1">
-        <v>-4.3994591713999998E-2</v>
+        <v>0.89069982777941503</v>
       </c>
       <c r="J2" s="1">
-        <v>0.67369008102500005</v>
+        <v>1.7250641007880501</v>
       </c>
       <c r="K2" s="1">
-        <v>1.3913747537650001</v>
+        <v>2.4007236565155301</v>
       </c>
       <c r="L2" s="1">
+        <v>4.6496048013039299</v>
+      </c>
+      <c r="M2" s="1">
+        <v>9.0051284118666697</v>
+      </c>
+      <c r="N2" s="1">
         <v>75</v>
       </c>
-      <c r="M2" s="1">
+      <c r="O2" s="1">
         <v>100</v>
       </c>
-      <c r="N2" s="1">
+      <c r="P2" s="1">
         <v>375</v>
       </c>
-      <c r="O2" s="1">
-        <v>-4.3994591713999998E-2</v>
+      <c r="Q2" s="2">
+        <v>2.4007236565155301</v>
+      </c>
+      <c r="R2" s="1">
+        <f>LOG(I2*0.4,10)</f>
+        <v>-0.44820864032900021</v>
+      </c>
+      <c r="S2" s="1">
+        <f t="shared" ref="S2:V2" si="0">LOG(J2*0.4,10)</f>
+        <v>-0.16113477123300041</v>
+      </c>
+      <c r="T2" s="1">
+        <f t="shared" si="0"/>
+        <v>-1.7597836685600238E-2</v>
+      </c>
+      <c r="U2" s="1">
+        <f t="shared" si="0"/>
+        <v>0.26947603240999995</v>
+      </c>
+      <c r="V2" s="1">
+        <f t="shared" si="0"/>
+        <v>0.55654990150599948</v>
+      </c>
+      <c r="W2" s="1">
+        <f t="shared" ref="W2" si="1">LOG(N2*0.4,10)</f>
+        <v>1.4771212547196624</v>
+      </c>
+      <c r="X2" s="1">
+        <f t="shared" ref="X2" si="2">LOG(O2*0.4,10)</f>
+        <v>1.6020599913279623</v>
+      </c>
+      <c r="Y2" s="1">
+        <f t="shared" ref="Y2" si="3">LOG(P2*0.4,10)</f>
+        <v>2.1760912590556809</v>
+      </c>
+      <c r="AA2" s="3">
+        <f>POWER(10,W2)</f>
+        <v>30.000000000000004</v>
+      </c>
+      <c r="AB2" s="3">
+        <f t="shared" ref="AB2:AC2" si="4">POWER(10,X2)</f>
+        <v>40</v>
+      </c>
+      <c r="AC2" s="3">
+        <f t="shared" si="4"/>
+        <v>149.99999999999997</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -545,43 +679,78 @@
         <v>17</v>
       </c>
       <c r="D3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E3" t="s">
         <v>19</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>2171</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="G3" s="1">
-        <v>-1.1205216008225001</v>
-      </c>
-      <c r="H3" s="1">
-        <v>-0.40283692808249999</v>
-      </c>
-      <c r="I3" s="1">
-        <v>-4.3994591713999998E-2</v>
-      </c>
-      <c r="J3" s="1">
-        <v>0.67369008102500005</v>
-      </c>
-      <c r="K3" s="1">
-        <v>1.3913747537650001</v>
-      </c>
-      <c r="L3" s="1">
-        <v>75</v>
-      </c>
-      <c r="M3" s="1">
-        <v>100</v>
+      <c r="H3" s="1" t="s">
+        <v>29</v>
       </c>
       <c r="N3" s="1">
-        <v>375</v>
+        <v>0</v>
       </c>
       <c r="O3" s="1">
-        <v>1000000000000</v>
+        <v>2.5</v>
+      </c>
+      <c r="P3" s="1">
+        <v>12.5</v>
+      </c>
+      <c r="Q3" s="2">
+        <v>2.5</v>
+      </c>
+      <c r="R3" s="1" t="e">
+        <f t="shared" ref="R3:R15" si="5">LOG(I3*0.4,10)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="S3" s="1" t="e">
+        <f t="shared" ref="S3:S15" si="6">LOG(J3*0.4,10)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="T3" s="1" t="e">
+        <f t="shared" ref="T3:T15" si="7">LOG(K3*0.4,10)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="U3" s="1" t="e">
+        <f t="shared" ref="U3:U15" si="8">LOG(L3*0.4,10)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="V3" s="1" t="e">
+        <f t="shared" ref="V3:V15" si="9">LOG(M3*0.4,10)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="W3" s="1" t="e">
+        <f t="shared" ref="W3:W15" si="10">LOG(N3*0.4,10)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="X3" s="1">
+        <f t="shared" ref="X3:X15" si="11">LOG(O3*0.4,10)</f>
+        <v>0</v>
+      </c>
+      <c r="Y3" s="1">
+        <f t="shared" ref="Y3:Y15" si="12">LOG(P3*0.4,10)</f>
+        <v>0.69897000433601875</v>
+      </c>
+      <c r="AA3" s="1">
+        <f>POWER(10,-0.7)</f>
+        <v>0.19952623149688795</v>
+      </c>
+      <c r="AB3" s="3">
+        <f t="shared" ref="AB3:AB11" si="13">POWER(10,X3)</f>
+        <v>1</v>
+      </c>
+      <c r="AC3" s="3">
+        <f t="shared" ref="AC3:AC11" si="14">POWER(10,Y3)</f>
+        <v>4.9999999999999991</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -592,43 +761,78 @@
         <v>17</v>
       </c>
       <c r="D4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E4" t="s">
         <v>20</v>
       </c>
-      <c r="E4">
+      <c r="F4">
         <v>2171</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="G4" s="1">
-        <v>-1.1205216008225001</v>
-      </c>
-      <c r="H4" s="1">
-        <v>-0.40283692808249999</v>
-      </c>
-      <c r="I4" s="1">
-        <v>-4.3994591713999998E-2</v>
-      </c>
-      <c r="J4" s="1">
-        <v>0.67369008102500005</v>
-      </c>
-      <c r="K4" s="1">
-        <v>1.3913747537650001</v>
-      </c>
-      <c r="L4" s="1">
-        <v>75</v>
-      </c>
-      <c r="M4" s="1">
-        <v>100</v>
+      <c r="H4" s="1" t="s">
+        <v>29</v>
       </c>
       <c r="N4" s="1">
-        <v>375</v>
+        <v>0</v>
       </c>
       <c r="O4" s="1">
-        <v>1000000000000</v>
+        <v>2500</v>
+      </c>
+      <c r="P4" s="1">
+        <v>12500</v>
+      </c>
+      <c r="Q4" s="2">
+        <v>2500</v>
+      </c>
+      <c r="R4" s="1" t="e">
+        <f t="shared" si="5"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="S4" s="1" t="e">
+        <f t="shared" si="6"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="T4" s="1" t="e">
+        <f t="shared" si="7"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="U4" s="1" t="e">
+        <f t="shared" si="8"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="V4" s="1" t="e">
+        <f t="shared" si="9"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="W4" s="1" t="e">
+        <f t="shared" si="10"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="X4" s="1">
+        <f t="shared" si="11"/>
+        <v>2.9999999999999996</v>
+      </c>
+      <c r="Y4" s="1">
+        <f t="shared" si="12"/>
+        <v>3.6989700043360187</v>
+      </c>
+      <c r="AA4" s="3" t="e">
+        <f t="shared" ref="AA3:AA11" si="15">POWER(10,W4)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="AB4" s="3">
+        <f t="shared" si="13"/>
+        <v>999.99999999999977</v>
+      </c>
+      <c r="AC4" s="3">
+        <f t="shared" si="14"/>
+        <v>5000.0000000000036</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -639,43 +843,78 @@
         <v>17</v>
       </c>
       <c r="D5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E5" t="s">
         <v>21</v>
       </c>
-      <c r="E5">
+      <c r="F5">
         <v>2171</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="G5" s="1">
-        <v>-1.1205216008225001</v>
-      </c>
-      <c r="H5" s="1">
-        <v>-0.40283692808249999</v>
-      </c>
-      <c r="I5" s="1">
-        <v>-4.3994591713999998E-2</v>
-      </c>
-      <c r="J5" s="1">
-        <v>0.67369008102500005</v>
-      </c>
-      <c r="K5" s="1">
-        <v>1.3913747537650001</v>
-      </c>
-      <c r="L5" s="1">
-        <v>75</v>
-      </c>
-      <c r="M5" s="1">
-        <v>100</v>
+      <c r="H5" s="1" t="s">
+        <v>29</v>
       </c>
       <c r="N5" s="1">
-        <v>375</v>
+        <v>2.5</v>
       </c>
       <c r="O5" s="1">
-        <v>1000000000000</v>
+        <v>25</v>
+      </c>
+      <c r="P5" s="1">
+        <v>125</v>
+      </c>
+      <c r="Q5" s="2">
+        <v>25</v>
+      </c>
+      <c r="R5" s="1" t="e">
+        <f t="shared" si="5"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="S5" s="1" t="e">
+        <f t="shared" si="6"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="T5" s="1" t="e">
+        <f t="shared" si="7"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="U5" s="1" t="e">
+        <f t="shared" si="8"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="V5" s="1" t="e">
+        <f t="shared" si="9"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="W5" s="1">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="X5" s="1">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+      <c r="Y5" s="1">
+        <f t="shared" si="12"/>
+        <v>1.6989700043360185</v>
+      </c>
+      <c r="AA5" s="3">
+        <f t="shared" si="15"/>
+        <v>1</v>
+      </c>
+      <c r="AB5" s="3">
+        <f t="shared" si="13"/>
+        <v>10</v>
+      </c>
+      <c r="AC5" s="3">
+        <f t="shared" si="14"/>
+        <v>49.999999999999993</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -686,43 +925,93 @@
         <v>17</v>
       </c>
       <c r="D6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E6" t="s">
         <v>22</v>
       </c>
-      <c r="E6">
+      <c r="F6">
         <v>2171</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="G6" s="1">
-        <v>-2.5723636382518301E-5</v>
-      </c>
-      <c r="H6" s="1">
-        <v>-9.2478633627754806E-6</v>
+      <c r="H6" s="1" t="s">
+        <v>29</v>
       </c>
       <c r="I6" s="1">
-        <v>-1.0099768529384699E-6</v>
+        <v>2.0447654448563199E-5</v>
       </c>
       <c r="J6" s="1">
-        <v>1.54657961667814E-5</v>
+        <v>3.9602022515795399E-5</v>
       </c>
       <c r="K6" s="1">
-        <v>3.19415691865243E-5</v>
+        <v>5.5113031600448297E-5</v>
       </c>
       <c r="L6" s="1">
+        <v>1.0674023878108101E-4</v>
+      </c>
+      <c r="M6" s="1">
+        <v>2.0672930238445E-4</v>
+      </c>
+      <c r="N6" s="1">
         <v>1.72176308539944E-3</v>
       </c>
-      <c r="M6" s="1">
+      <c r="O6" s="1">
         <v>2.2956841138659298E-3</v>
       </c>
-      <c r="N6" s="1">
+      <c r="P6" s="1">
         <v>8.6088154269972402E-3</v>
       </c>
-      <c r="O6" s="1">
-        <v>-1.0099768529384699E-6</v>
+      <c r="Q6" s="2">
+        <v>5.5113031600448297E-5</v>
+      </c>
+      <c r="R6" s="1">
+        <f>LOG(I6*43560*0.4,10)</f>
+        <v>-0.44820864032900126</v>
+      </c>
+      <c r="S6" s="1">
+        <f t="shared" ref="S6:V6" si="16">LOG(J6*43560*0.4,10)</f>
+        <v>-0.16113477123300105</v>
+      </c>
+      <c r="T6" s="1">
+        <f t="shared" si="16"/>
+        <v>-1.7597836685600637E-2</v>
+      </c>
+      <c r="U6" s="1">
+        <f t="shared" si="16"/>
+        <v>0.26947603240999601</v>
+      </c>
+      <c r="V6" s="1">
+        <f t="shared" si="16"/>
+        <v>0.55654990150599826</v>
+      </c>
+      <c r="W6" s="1">
+        <f t="shared" si="10"/>
+        <v>-3.1619666163640767</v>
+      </c>
+      <c r="X6" s="1">
+        <f t="shared" si="11"/>
+        <v>-3.037027879755775</v>
+      </c>
+      <c r="Y6" s="1">
+        <f t="shared" si="12"/>
+        <v>-2.4629966120280562</v>
+      </c>
+      <c r="AA6" s="3">
+        <f t="shared" si="15"/>
+        <v>6.8870523415977606E-4</v>
+      </c>
+      <c r="AB6" s="3">
+        <f t="shared" si="13"/>
+        <v>9.1827364554637205E-4</v>
+      </c>
+      <c r="AC6" s="3">
+        <f t="shared" si="14"/>
+        <v>3.4435261707988956E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -733,90 +1022,175 @@
         <v>17</v>
       </c>
       <c r="D7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E7" t="s">
         <v>23</v>
       </c>
-      <c r="E7">
+      <c r="F7">
         <v>2171</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="G7" s="1">
-        <v>-2.5723636382518301E-5</v>
-      </c>
-      <c r="H7" s="1">
-        <v>-9.2478633627754806E-6</v>
-      </c>
-      <c r="I7" s="1">
-        <v>-1.0099768529384699E-6</v>
-      </c>
-      <c r="J7" s="1">
-        <v>1.54657961667814E-5</v>
-      </c>
-      <c r="K7" s="1">
-        <v>3.19415691865243E-5</v>
-      </c>
-      <c r="L7" s="1">
-        <v>1.72176308539944E-3</v>
-      </c>
-      <c r="M7" s="1">
-        <v>2.2956841138659298E-3</v>
+      <c r="H7" s="1" t="s">
+        <v>29</v>
       </c>
       <c r="N7" s="1">
-        <v>8.6088154269972402E-3</v>
+        <v>5000</v>
       </c>
       <c r="O7" s="1">
-        <v>1000000000000</v>
+        <v>50000</v>
+      </c>
+      <c r="P7" s="1">
+        <v>250000</v>
+      </c>
+      <c r="Q7" s="2">
+        <v>50000</v>
+      </c>
+      <c r="R7" s="1" t="e">
+        <f t="shared" si="5"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="S7" s="1" t="e">
+        <f t="shared" si="6"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="T7" s="1" t="e">
+        <f t="shared" si="7"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="U7" s="1" t="e">
+        <f t="shared" si="8"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="V7" s="1" t="e">
+        <f t="shared" si="9"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="W7" s="1">
+        <f t="shared" si="10"/>
+        <v>3.3010299956639808</v>
+      </c>
+      <c r="X7" s="1">
+        <f t="shared" si="11"/>
+        <v>4.3010299956639804</v>
+      </c>
+      <c r="Y7" s="1">
+        <f t="shared" si="12"/>
+        <v>5</v>
+      </c>
+      <c r="AA7" s="3">
+        <f t="shared" si="15"/>
+        <v>1999.9999999999998</v>
+      </c>
+      <c r="AB7" s="3">
+        <f t="shared" si="13"/>
+        <v>19999.999999999982</v>
+      </c>
+      <c r="AC7" s="3">
+        <f t="shared" si="14"/>
+        <v>100000</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E8" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="E8">
+      <c r="F8" s="4">
         <v>2171</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="G8" s="1">
-        <v>-7.2508415513499997</v>
-      </c>
-      <c r="H8" s="1">
-        <v>-7.2508415513499997</v>
-      </c>
-      <c r="I8" s="1">
-        <v>-7.2508415513499997</v>
-      </c>
-      <c r="J8" s="1">
-        <v>-7.2508415513499997</v>
-      </c>
-      <c r="K8" s="1">
-        <v>-7.2508415513499997</v>
-      </c>
-      <c r="L8" s="1">
+      <c r="H8" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="I8" s="5">
+        <v>3.1448750000050798E-3</v>
+      </c>
+      <c r="J8" s="5">
+        <v>3.1448750000050798E-3</v>
+      </c>
+      <c r="K8" s="5">
+        <v>3.1448750000050798E-3</v>
+      </c>
+      <c r="L8" s="5">
+        <v>3.1448750000050798E-3</v>
+      </c>
+      <c r="M8" s="5">
+        <v>3.1448750000050798E-3</v>
+      </c>
+      <c r="N8" s="5">
         <v>25</v>
       </c>
-      <c r="M8" s="1">
+      <c r="O8" s="5">
         <v>50</v>
       </c>
-      <c r="N8" s="1">
+      <c r="P8" s="5">
         <v>125</v>
       </c>
-      <c r="O8" s="1">
-        <v>-7.2508415513499997</v>
+      <c r="Q8" s="6">
+        <v>3.1448750000050798E-3</v>
+      </c>
+      <c r="R8" s="5">
+        <f t="shared" si="5"/>
+        <v>-2.9003366205399996</v>
+      </c>
+      <c r="S8" s="5">
+        <f t="shared" si="6"/>
+        <v>-2.9003366205399996</v>
+      </c>
+      <c r="T8" s="5">
+        <f t="shared" si="7"/>
+        <v>-2.9003366205399996</v>
+      </c>
+      <c r="U8" s="5">
+        <f t="shared" si="8"/>
+        <v>-2.9003366205399996</v>
+      </c>
+      <c r="V8" s="5">
+        <f t="shared" si="9"/>
+        <v>-2.9003366205399996</v>
+      </c>
+      <c r="W8" s="5">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+      <c r="X8" s="5">
+        <f t="shared" si="11"/>
+        <v>1.301029995663981</v>
+      </c>
+      <c r="Y8" s="5">
+        <f t="shared" si="12"/>
+        <v>1.6989700043360185</v>
+      </c>
+      <c r="AA8" s="3">
+        <f t="shared" si="15"/>
+        <v>10</v>
+      </c>
+      <c r="AB8" s="3">
+        <f t="shared" si="13"/>
+        <v>19.999999999999996</v>
+      </c>
+      <c r="AC8" s="3">
+        <f t="shared" si="14"/>
+        <v>49.999999999999993</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -827,43 +1201,93 @@
         <v>17</v>
       </c>
       <c r="D9" t="s">
+        <v>30</v>
+      </c>
+      <c r="E9" t="s">
         <v>16</v>
       </c>
-      <c r="E9">
+      <c r="F9">
         <v>2171</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="G9" s="1">
-        <v>4.5470917846249996</v>
-      </c>
-      <c r="H9" s="1">
-        <v>7.1958933108999998</v>
+      <c r="H9" s="1" t="s">
+        <v>29</v>
       </c>
       <c r="I9" s="1">
-        <v>8.5202940740499997</v>
+        <v>164.73152636503099</v>
       </c>
       <c r="J9" s="1">
-        <v>11.169095600325001</v>
+        <v>1889.2843758869601</v>
       </c>
       <c r="K9" s="1">
-        <v>13.8178971266</v>
+        <v>6398.1974485122601</v>
       </c>
       <c r="L9" s="1">
+        <v>73380.091473977998</v>
+      </c>
+      <c r="M9" s="1">
+        <v>841586.69188638905</v>
+      </c>
+      <c r="N9" s="1">
         <v>325</v>
       </c>
-      <c r="M9" s="1">
+      <c r="O9" s="1">
         <v>750</v>
       </c>
-      <c r="N9" s="1">
+      <c r="P9" s="1">
         <v>25000</v>
       </c>
-      <c r="O9" s="1">
-        <v>4.5470917846249996</v>
+      <c r="Q9" s="2">
+        <v>164.73152636503099</v>
+      </c>
+      <c r="R9" s="1">
+        <f t="shared" si="5"/>
+        <v>1.8188367138499972</v>
+      </c>
+      <c r="S9" s="1">
+        <f t="shared" si="6"/>
+        <v>2.8783573243599991</v>
+      </c>
+      <c r="T9" s="1">
+        <f t="shared" si="7"/>
+        <v>3.4081176296199995</v>
+      </c>
+      <c r="U9" s="1">
+        <f t="shared" si="8"/>
+        <v>4.4676382401299994</v>
+      </c>
+      <c r="V9" s="1">
+        <f t="shared" si="9"/>
+        <v>5.5271588506399993</v>
+      </c>
+      <c r="W9" s="1">
+        <f t="shared" si="10"/>
+        <v>2.1139433523068365</v>
+      </c>
+      <c r="X9" s="1">
+        <f t="shared" si="11"/>
+        <v>2.4771212547196622</v>
+      </c>
+      <c r="Y9" s="1">
+        <f t="shared" si="12"/>
+        <v>4</v>
+      </c>
+      <c r="AA9" s="3">
+        <f t="shared" si="15"/>
+        <v>129.99999999999997</v>
+      </c>
+      <c r="AB9" s="3">
+        <f t="shared" si="13"/>
+        <v>299.99999999999994</v>
+      </c>
+      <c r="AC9" s="3">
+        <f t="shared" si="14"/>
+        <v>10000</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>15</v>
       </c>
@@ -874,43 +1298,93 @@
         <v>17</v>
       </c>
       <c r="D10" t="s">
+        <v>30</v>
+      </c>
+      <c r="E10" t="s">
         <v>19</v>
       </c>
-      <c r="E10">
+      <c r="F10">
         <v>2171</v>
       </c>
-      <c r="F10" t="s">
+      <c r="G10" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="G10" s="1">
-        <v>274.87927769250001</v>
-      </c>
-      <c r="H10" s="1">
-        <v>385.58443571999999</v>
+      <c r="H10" s="1" t="s">
+        <v>29</v>
       </c>
       <c r="I10" s="1">
-        <v>440.93701473250002</v>
+        <v>2500000000000000</v>
       </c>
       <c r="J10" s="1">
-        <v>551.64217275999999</v>
+        <v>2500000000000000</v>
       </c>
       <c r="K10" s="1">
-        <v>662.34733078750003</v>
+        <v>2500000000000000</v>
       </c>
       <c r="L10" s="1">
+        <v>2500000000000000</v>
+      </c>
+      <c r="M10" s="1">
+        <v>2500000000000000</v>
+      </c>
+      <c r="N10" s="1">
         <v>50</v>
-      </c>
-      <c r="M10" s="1">
-        <v>250</v>
-      </c>
-      <c r="N10" s="1">
-        <v>500</v>
       </c>
       <c r="O10" s="1">
         <v>250</v>
       </c>
+      <c r="P10" s="1">
+        <v>500</v>
+      </c>
+      <c r="Q10" s="2">
+        <v>250</v>
+      </c>
+      <c r="R10" s="1">
+        <f t="shared" si="5"/>
+        <v>14.999999999999998</v>
+      </c>
+      <c r="S10" s="1">
+        <f t="shared" si="6"/>
+        <v>14.999999999999998</v>
+      </c>
+      <c r="T10" s="1">
+        <f t="shared" si="7"/>
+        <v>14.999999999999998</v>
+      </c>
+      <c r="U10" s="1">
+        <f t="shared" si="8"/>
+        <v>14.999999999999998</v>
+      </c>
+      <c r="V10" s="1">
+        <f t="shared" si="9"/>
+        <v>14.999999999999998</v>
+      </c>
+      <c r="W10" s="1">
+        <f t="shared" si="10"/>
+        <v>1.301029995663981</v>
+      </c>
+      <c r="X10" s="1">
+        <f t="shared" si="11"/>
+        <v>2</v>
+      </c>
+      <c r="Y10" s="1">
+        <f t="shared" si="12"/>
+        <v>2.3010299956639808</v>
+      </c>
+      <c r="AA10" s="3">
+        <f t="shared" si="15"/>
+        <v>19.999999999999996</v>
+      </c>
+      <c r="AB10" s="3">
+        <f t="shared" si="13"/>
+        <v>100</v>
+      </c>
+      <c r="AC10" s="3">
+        <f t="shared" si="14"/>
+        <v>199.99999999999991</v>
+      </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -921,43 +1395,93 @@
         <v>17</v>
       </c>
       <c r="D11" t="s">
+        <v>30</v>
+      </c>
+      <c r="E11" t="s">
         <v>20</v>
       </c>
-      <c r="E11">
+      <c r="F11">
         <v>2171</v>
       </c>
-      <c r="F11" t="s">
+      <c r="G11" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="G11" s="1">
-        <v>274879.27769249998</v>
-      </c>
-      <c r="H11" s="1">
-        <v>385584.43572000001</v>
+      <c r="H11" s="1" t="s">
+        <v>29</v>
       </c>
       <c r="I11" s="1">
-        <v>440937.01473250001</v>
+        <v>2.5E+18</v>
       </c>
       <c r="J11" s="1">
-        <v>551642.17275999999</v>
+        <v>2.5E+18</v>
       </c>
       <c r="K11" s="1">
-        <v>662347.33078750002</v>
+        <v>2.5E+18</v>
       </c>
       <c r="L11" s="1">
+        <v>2.5E+18</v>
+      </c>
+      <c r="M11" s="1">
+        <v>2.5E+18</v>
+      </c>
+      <c r="N11" s="1">
         <v>50000</v>
-      </c>
-      <c r="M11" s="1">
-        <v>250000</v>
-      </c>
-      <c r="N11" s="1">
-        <v>500000</v>
       </c>
       <c r="O11" s="1">
         <v>250000</v>
       </c>
+      <c r="P11" s="1">
+        <v>500000</v>
+      </c>
+      <c r="Q11" s="2">
+        <v>250000</v>
+      </c>
+      <c r="R11" s="1">
+        <f t="shared" si="5"/>
+        <v>17.999999999999996</v>
+      </c>
+      <c r="S11" s="1">
+        <f t="shared" si="6"/>
+        <v>17.999999999999996</v>
+      </c>
+      <c r="T11" s="1">
+        <f t="shared" si="7"/>
+        <v>17.999999999999996</v>
+      </c>
+      <c r="U11" s="1">
+        <f t="shared" si="8"/>
+        <v>17.999999999999996</v>
+      </c>
+      <c r="V11" s="1">
+        <f t="shared" si="9"/>
+        <v>17.999999999999996</v>
+      </c>
+      <c r="W11" s="1">
+        <f t="shared" si="10"/>
+        <v>4.3010299956639804</v>
+      </c>
+      <c r="X11" s="1">
+        <f t="shared" si="11"/>
+        <v>5</v>
+      </c>
+      <c r="Y11" s="1">
+        <f t="shared" si="12"/>
+        <v>5.3010299956639813</v>
+      </c>
+      <c r="AA11" s="3">
+        <f t="shared" si="15"/>
+        <v>19999.999999999982</v>
+      </c>
+      <c r="AB11" s="3">
+        <f t="shared" si="13"/>
+        <v>100000</v>
+      </c>
+      <c r="AC11" s="3">
+        <f t="shared" si="14"/>
+        <v>200000.00000000041</v>
+      </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>15</v>
       </c>
@@ -968,43 +1492,78 @@
         <v>17</v>
       </c>
       <c r="D12" t="s">
+        <v>30</v>
+      </c>
+      <c r="E12" t="s">
         <v>21</v>
       </c>
-      <c r="E12">
+      <c r="F12">
         <v>2171</v>
       </c>
-      <c r="F12" t="s">
+      <c r="G12" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="G12" s="1">
-        <v>274879.27769249998</v>
-      </c>
-      <c r="H12" s="1">
-        <v>385584.43572000001</v>
-      </c>
-      <c r="I12" s="1">
-        <v>440937.01473250001</v>
-      </c>
-      <c r="J12" s="1">
-        <v>551642.17275999999</v>
-      </c>
-      <c r="K12" s="1">
-        <v>662347.33078750002</v>
-      </c>
-      <c r="L12" s="1">
-        <v>50000</v>
-      </c>
-      <c r="M12" s="1">
-        <v>250000</v>
+      <c r="H12" s="1" t="s">
+        <v>29</v>
       </c>
       <c r="N12" s="1">
-        <v>500000</v>
+        <v>2.5</v>
       </c>
       <c r="O12" s="1">
-        <v>1000000000000</v>
+        <v>5</v>
+      </c>
+      <c r="P12" s="1">
+        <v>25</v>
+      </c>
+      <c r="Q12" s="2">
+        <v>5</v>
+      </c>
+      <c r="R12" s="1" t="e">
+        <f t="shared" si="5"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="S12" s="1" t="e">
+        <f t="shared" si="6"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="T12" s="1" t="e">
+        <f t="shared" si="7"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="U12" s="1" t="e">
+        <f t="shared" si="8"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="V12" s="1" t="e">
+        <f t="shared" si="9"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="W12" s="1">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="X12" s="1">
+        <f t="shared" si="11"/>
+        <v>0.30102999566398114</v>
+      </c>
+      <c r="Y12" s="1">
+        <f t="shared" si="12"/>
+        <v>1</v>
+      </c>
+      <c r="AA12" s="3">
+        <f t="shared" ref="AA12:AA15" si="17">POWER(10,W12)</f>
+        <v>1</v>
+      </c>
+      <c r="AB12" s="3">
+        <f t="shared" ref="AB12:AB15" si="18">POWER(10,X12)</f>
+        <v>2</v>
+      </c>
+      <c r="AC12" s="3">
+        <f t="shared" ref="AC12:AC15" si="19">POWER(10,Y12)</f>
+        <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>15</v>
       </c>
@@ -1015,43 +1574,93 @@
         <v>17</v>
       </c>
       <c r="D13" t="s">
+        <v>30</v>
+      </c>
+      <c r="E13" t="s">
         <v>22</v>
       </c>
-      <c r="E13">
+      <c r="F13">
         <v>2171</v>
       </c>
-      <c r="F13" t="s">
+      <c r="G13" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="G13" s="1">
-        <v>1.04386863742539E-4</v>
-      </c>
-      <c r="H13" s="1">
-        <v>1.6519497958907201E-4</v>
+      <c r="H13" s="1" t="s">
+        <v>29</v>
       </c>
       <c r="I13" s="1">
-        <v>1.95599037512626E-4</v>
+        <v>3.7817154812909001E-3</v>
       </c>
       <c r="J13" s="1">
-        <v>2.5640715335915898E-4</v>
+        <v>4.3372001282988099E-2</v>
       </c>
       <c r="K13" s="1">
-        <v>3.1721526920569298E-4</v>
+        <v>0.146882402399271</v>
       </c>
       <c r="L13" s="1">
+        <v>1.6845751027083999</v>
+      </c>
+      <c r="M13" s="1">
+        <v>19.320171990045601</v>
+      </c>
+      <c r="N13" s="1">
         <v>7.4609733700642701E-3</v>
       </c>
-      <c r="M13" s="1">
+      <c r="O13" s="1">
         <v>1.7217630853994401E-2</v>
       </c>
-      <c r="N13" s="1">
+      <c r="P13" s="1">
         <v>0.57392102846648296</v>
       </c>
-      <c r="O13" s="1">
-        <v>1.04386863742539E-4</v>
+      <c r="Q13" s="2">
+        <v>3.7817154812909001E-3</v>
+      </c>
+      <c r="R13" s="1">
+        <f>LOG(I13*43560*0.4,10)</f>
+        <v>1.8188367138499992</v>
+      </c>
+      <c r="S13" s="1">
+        <f t="shared" ref="S13:Y13" si="20">LOG(J13*43560*0.4,10)</f>
+        <v>2.8783573243599996</v>
+      </c>
+      <c r="T13" s="1">
+        <f t="shared" si="20"/>
+        <v>3.4081176296199982</v>
+      </c>
+      <c r="U13" s="1">
+        <f t="shared" si="20"/>
+        <v>4.4676382401299994</v>
+      </c>
+      <c r="V13" s="1">
+        <f t="shared" si="20"/>
+        <v>5.5271588506399976</v>
+      </c>
+      <c r="W13" s="1">
+        <f t="shared" si="20"/>
+        <v>2.1139433523068361</v>
+      </c>
+      <c r="X13" s="1">
+        <f t="shared" si="20"/>
+        <v>2.4771212547196599</v>
+      </c>
+      <c r="Y13" s="1">
+        <f t="shared" si="20"/>
+        <v>4</v>
+      </c>
+      <c r="AA13" s="3">
+        <f t="shared" si="17"/>
+        <v>129.99999999999986</v>
+      </c>
+      <c r="AB13" s="3">
+        <f t="shared" si="18"/>
+        <v>299.99999999999835</v>
+      </c>
+      <c r="AC13" s="3">
+        <f t="shared" si="19"/>
+        <v>10000</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -1062,43 +1671,78 @@
         <v>17</v>
       </c>
       <c r="D14" t="s">
+        <v>30</v>
+      </c>
+      <c r="E14" t="s">
         <v>23</v>
       </c>
-      <c r="E14">
+      <c r="F14">
         <v>2171</v>
       </c>
-      <c r="F14" t="s">
+      <c r="G14" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="G14" s="1">
-        <v>1.04386863742539E-4</v>
-      </c>
-      <c r="H14" s="1">
-        <v>1.6519497958907201E-4</v>
-      </c>
-      <c r="I14" s="1">
-        <v>1.95599037512626E-4</v>
-      </c>
-      <c r="J14" s="1">
-        <v>2.5640715335915898E-4</v>
-      </c>
-      <c r="K14" s="1">
-        <v>3.1721526920569298E-4</v>
-      </c>
-      <c r="L14" s="1">
-        <v>7.4609733700642701E-3</v>
-      </c>
-      <c r="M14" s="1">
-        <v>1.7217630853994401E-2</v>
+      <c r="H14" s="1" t="s">
+        <v>29</v>
       </c>
       <c r="N14" s="1">
-        <v>0.57392102846648296</v>
+        <v>5000</v>
       </c>
       <c r="O14" s="1">
-        <v>1000000000000</v>
+        <v>10000</v>
+      </c>
+      <c r="P14" s="1">
+        <v>50000</v>
+      </c>
+      <c r="Q14" s="2">
+        <v>10000</v>
+      </c>
+      <c r="R14" s="1" t="e">
+        <f t="shared" si="5"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="S14" s="1" t="e">
+        <f t="shared" si="6"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="T14" s="1" t="e">
+        <f t="shared" si="7"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="U14" s="1" t="e">
+        <f t="shared" si="8"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="V14" s="1" t="e">
+        <f t="shared" si="9"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="W14" s="1">
+        <f t="shared" si="10"/>
+        <v>3.3010299956639808</v>
+      </c>
+      <c r="X14" s="1">
+        <f t="shared" si="11"/>
+        <v>3.6020599913279621</v>
+      </c>
+      <c r="Y14" s="1">
+        <f t="shared" si="12"/>
+        <v>4.3010299956639804</v>
+      </c>
+      <c r="AA14" s="3">
+        <f t="shared" si="17"/>
+        <v>1999.9999999999998</v>
+      </c>
+      <c r="AB14" s="3">
+        <f t="shared" si="18"/>
+        <v>3999.9999999999995</v>
+      </c>
+      <c r="AC14" s="3">
+        <f t="shared" si="19"/>
+        <v>19999.999999999982</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>15</v>
       </c>
@@ -1109,40 +1753,90 @@
         <v>17</v>
       </c>
       <c r="D15" t="s">
+        <v>30</v>
+      </c>
+      <c r="E15" t="s">
         <v>24</v>
       </c>
-      <c r="E15">
+      <c r="F15">
         <v>2171</v>
       </c>
-      <c r="F15" t="s">
+      <c r="G15" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="G15" s="1">
-        <v>5.4836069437750004</v>
-      </c>
-      <c r="H15" s="1">
-        <v>8.1127840137750002</v>
+      <c r="H15" s="1" t="s">
+        <v>29</v>
       </c>
       <c r="I15" s="1">
-        <v>9.4273725487750006</v>
+        <v>390.28583217885699</v>
       </c>
       <c r="J15" s="1">
-        <v>12.056549618775</v>
+        <v>4395.9588073436798</v>
       </c>
       <c r="K15" s="1">
-        <v>14.685726688800001</v>
+        <v>14753.2950588318</v>
       </c>
       <c r="L15" s="1">
+        <v>166172.768786264</v>
+      </c>
+      <c r="M15" s="1">
+        <v>1871676.0545095101</v>
+      </c>
+      <c r="N15" s="1">
         <v>1250</v>
       </c>
-      <c r="M15" s="1">
+      <c r="O15" s="1">
         <v>2500</v>
       </c>
-      <c r="N15" s="1">
+      <c r="P15" s="1">
         <v>12500</v>
       </c>
-      <c r="O15" s="1">
-        <v>12.056549618775</v>
+      <c r="Q15" s="2">
+        <v>2500</v>
+      </c>
+      <c r="R15" s="1">
+        <f t="shared" si="5"/>
+        <v>2.1934427775099996</v>
+      </c>
+      <c r="S15" s="1">
+        <f t="shared" si="6"/>
+        <v>3.2451136055099989</v>
+      </c>
+      <c r="T15" s="1">
+        <f t="shared" si="7"/>
+        <v>3.7709490195099971</v>
+      </c>
+      <c r="U15" s="1">
+        <f t="shared" si="8"/>
+        <v>4.8226198475099977</v>
+      </c>
+      <c r="V15" s="1">
+        <f t="shared" si="9"/>
+        <v>5.8742906755199984</v>
+      </c>
+      <c r="W15" s="1">
+        <f t="shared" si="10"/>
+        <v>2.6989700043360183</v>
+      </c>
+      <c r="X15" s="1">
+        <f t="shared" si="11"/>
+        <v>2.9999999999999996</v>
+      </c>
+      <c r="Y15" s="1">
+        <f t="shared" si="12"/>
+        <v>3.6989700043360187</v>
+      </c>
+      <c r="AA15" s="3">
+        <f t="shared" si="17"/>
+        <v>499.99999999999983</v>
+      </c>
+      <c r="AB15" s="3">
+        <f t="shared" si="18"/>
+        <v>999.99999999999977</v>
+      </c>
+      <c r="AC15" s="3">
+        <f t="shared" si="19"/>
+        <v>5000.0000000000036</v>
       </c>
     </row>
   </sheetData>

</xml_diff>